<commit_message>
added code to generate plots
added both plots, and code to generate plots.
</commit_message>
<xml_diff>
--- a/diagnostic comparisons/diagnostic_comparisons_5_sigma.xlsx
+++ b/diagnostic comparisons/diagnostic_comparisons_5_sigma.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mitchell\Documents\GitHub\astrophysicscapstone\diagnostic comparisons\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5b824f7673720fc0/Documents/GitHub/astrophysicscapstone/diagnostic comparisons/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4DA423D8-CB58-4F19-9A6D-E5F60B5AA5B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="8_{4DA423D8-CB58-4F19-9A6D-E5F60B5AA5B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9CC4CD1-942E-4D67-A4B9-C1A525C08CF8}"/>
   <bookViews>
-    <workbookView xWindow="3915" yWindow="4125" windowWidth="20985" windowHeight="15585"/>
+    <workbookView xWindow="35880" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="diagnostic_comparisons_5_sigma" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="11">
   <si>
     <t>Lacy Completeness (%)</t>
   </si>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1220,6 +1220,1185 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-AU" b="1" i="1" u="sng"/>
+              <a:t>Selection</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-AU" b="1" i="1" u="sng" baseline="0"/>
+              <a:t> Reliability</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-AU" b="1" i="1" u="sng"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12830537443611298"/>
+          <c:y val="0.18669411790611423"/>
+          <c:w val="0.73922706600410382"/>
+          <c:h val="0.51883432369603988"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>diagnostic_comparisons_5_sigma!$M$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lacy Reliability (%)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>diagnostic_comparisons_5_sigma!$L$21:$L$23</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>CDFS</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>COSMOS</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>UDS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>diagnostic_comparisons_5_sigma!$M$21:$M$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>11.56</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.62</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.8000000000000007</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-306F-41B9-A5EE-2F85250BC0A5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>diagnostic_comparisons_5_sigma!$N$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Donley Reliability (%)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>diagnostic_comparisons_5_sigma!$L$21:$L$23</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>CDFS</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>COSMOS</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>UDS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>diagnostic_comparisons_5_sigma!$N$21:$N$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>30.08</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>39.22</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20.51</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-306F-41B9-A5EE-2F85250BC0A5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>diagnostic_comparisons_5_sigma!$O$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Messias Reliability (%)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>diagnostic_comparisons_5_sigma!$L$21:$L$23</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>CDFS</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>COSMOS</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>UDS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>diagnostic_comparisons_5_sigma!$O$21:$O$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>42.22</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.81</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-306F-41B9-A5EE-2F85250BC0A5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>diagnostic_comparisons_5_sigma!$P$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Szokoly Reliability (%)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>diagnostic_comparisons_5_sigma!$L$21:$L$23</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>CDFS</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>COSMOS</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>UDS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>diagnostic_comparisons_5_sigma!$P$21:$P$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>24.09</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-306F-41B9-A5EE-2F85250BC0A5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="889822352"/>
+        <c:axId val="989362608"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="4"/>
+                <c:order val="4"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>diagnostic_comparisons_5_sigma!$Q$20</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent5"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>diagnostic_comparisons_5_sigma!$L$21:$L$23</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="3"/>
+                      <c:pt idx="0">
+                        <c:v>CDFS</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>COSMOS</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>UDS</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>diagnostic_comparisons_5_sigma!$Q$21:$Q$23</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="3"/>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000004-306F-41B9-A5EE-2F85250BC0A5}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="889822352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="989362608"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="989362608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="889822352"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.13831171659918531"/>
+          <c:y val="0.80586715193915004"/>
+          <c:w val="0.666233697971919"/>
+          <c:h val="0.13920153383013995"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-AU" b="1" i="1" u="sng"/>
+              <a:t>Selection</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-AU" b="1" i="1" u="sng" baseline="0"/>
+              <a:t> Completeness</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-AU" b="1" i="1" u="sng"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11343094443439035"/>
+          <c:y val="0.18452743547124045"/>
+          <c:w val="0.77191109863579999"/>
+          <c:h val="0.52468387381355974"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>diagnostic_comparisons_5_sigma!$M$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lacy Completeness (%)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>diagnostic_comparisons_5_sigma!$L$15:$L$17</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>CDFS</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>COSMOS</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>UDS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>diagnostic_comparisons_5_sigma!$M$15:$M$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>98.06</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>96.55</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>94.29</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AA38-4A99-91E9-E350EEA380A1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>diagnostic_comparisons_5_sigma!$N$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Donley Completeness (%)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>diagnostic_comparisons_5_sigma!$L$15:$L$17</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>CDFS</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>COSMOS</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>UDS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>diagnostic_comparisons_5_sigma!$N$15:$N$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>35.92</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>68.97</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45.71</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-AA38-4A99-91E9-E350EEA380A1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>diagnostic_comparisons_5_sigma!$O$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Messias Completeness (%)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>diagnostic_comparisons_5_sigma!$L$15:$L$17</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>CDFS</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>COSMOS</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>UDS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>diagnostic_comparisons_5_sigma!$O$15:$O$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>18.45</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44.83</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22.86</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-AA38-4A99-91E9-E350EEA380A1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>diagnostic_comparisons_5_sigma!$P$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Szokoly Completeness (%)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>diagnostic_comparisons_5_sigma!$L$15:$L$17</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>CDFS</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>COSMOS</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>UDS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>diagnostic_comparisons_5_sigma!$P$15:$P$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>24.26</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-AA38-4A99-91E9-E350EEA380A1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="889815632"/>
+        <c:axId val="867705888"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="889815632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="867705888"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="867705888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="889815632"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.17239915414108509"/>
+          <c:y val="0.82462562174388754"/>
+          <c:w val="0.60569030122541201"/>
+          <c:h val="0.13557336763950625"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1300,6 +2479,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -1804,6 +3063,1012 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2375,6 +4640,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42A35688-C918-EA85-A117-18AAFE7A7821}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>606425</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E83C03F-E79B-E8A9-B74D-B4DED537D3F5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2679,16 +5016,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="AA17" sqref="AA17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2714,7 +5051,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -2743,7 +5080,7 @@
         <v>24.09</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -2766,7 +5103,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -2789,7 +5126,7 @@
         <v>14.81</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>0</v>
       </c>
@@ -2815,7 +5152,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -2844,7 +5181,7 @@
         <v>24.09</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -2867,7 +5204,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -2887,6 +5224,122 @@
         <v>22.86</v>
       </c>
       <c r="G14">
+        <v>14.81</v>
+      </c>
+      <c r="M14" t="s">
+        <v>0</v>
+      </c>
+      <c r="N14" t="s">
+        <v>2</v>
+      </c>
+      <c r="O14" t="s">
+        <v>4</v>
+      </c>
+      <c r="P14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="L15" t="s">
+        <v>8</v>
+      </c>
+      <c r="M15">
+        <v>98.06</v>
+      </c>
+      <c r="N15">
+        <v>35.92</v>
+      </c>
+      <c r="O15">
+        <v>18.45</v>
+      </c>
+      <c r="P15">
+        <v>24.26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="L16" t="s">
+        <v>9</v>
+      </c>
+      <c r="M16">
+        <v>96.55</v>
+      </c>
+      <c r="N16">
+        <v>68.97</v>
+      </c>
+      <c r="O16">
+        <v>44.83</v>
+      </c>
+    </row>
+    <row r="17" spans="12:16" x14ac:dyDescent="0.35">
+      <c r="L17" t="s">
+        <v>10</v>
+      </c>
+      <c r="M17">
+        <v>94.29</v>
+      </c>
+      <c r="N17">
+        <v>45.71</v>
+      </c>
+      <c r="O17">
+        <v>22.86</v>
+      </c>
+    </row>
+    <row r="20" spans="12:16" x14ac:dyDescent="0.35">
+      <c r="M20" t="s">
+        <v>1</v>
+      </c>
+      <c r="N20" t="s">
+        <v>3</v>
+      </c>
+      <c r="O20" t="s">
+        <v>5</v>
+      </c>
+      <c r="P20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="12:16" x14ac:dyDescent="0.35">
+      <c r="L21" t="s">
+        <v>8</v>
+      </c>
+      <c r="M21">
+        <v>11.56</v>
+      </c>
+      <c r="N21">
+        <v>30.08</v>
+      </c>
+      <c r="O21">
+        <v>42.22</v>
+      </c>
+      <c r="P21">
+        <v>24.09</v>
+      </c>
+    </row>
+    <row r="22" spans="12:16" x14ac:dyDescent="0.35">
+      <c r="L22" t="s">
+        <v>9</v>
+      </c>
+      <c r="M22">
+        <v>11.62</v>
+      </c>
+      <c r="N22">
+        <v>39.22</v>
+      </c>
+      <c r="O22">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="12:16" x14ac:dyDescent="0.35">
+      <c r="L23" t="s">
+        <v>10</v>
+      </c>
+      <c r="M23">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="N23">
+        <v>20.51</v>
+      </c>
+      <c r="O23">
         <v>14.81</v>
       </c>
     </row>

</xml_diff>